<commit_message>
04/10- Market factors redone
</commit_message>
<xml_diff>
--- a/Manufacturing.xlsx
+++ b/Manufacturing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucar\PycharmProjects\NJORD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucar\PycharmProjects\NJORD_2022_Albin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:1_{6D50E043-E026-4E9B-85B5-023CC1E6505C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E8FD64D-A233-4EA4-A800-ADBFB4C57EEC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F22FFAAD-A141-4B9A-A1C3-56190C62D5AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9972" yWindow="720" windowWidth="15360" windowHeight="11292" xr2:uid="{25E8C77A-571D-440B-A5FA-B562A92F21E1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{25E8C77A-571D-440B-A5FA-B562A92F21E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -171,9 +171,18 @@
     </comment>
     <comment ref="O52" authorId="4" shapeId="0" xr:uid="{EEC4A3A6-629D-4FD1-A07D-AE48AE659198}">
       <text>
-        <t xml:space="preserve">Njord:
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">Njord:
 eller 450
 </t>
+        </r>
       </text>
     </comment>
     <comment ref="N71" authorId="2" shapeId="0" xr:uid="{F4560A1B-ADF0-4B1C-BDB7-00965A4A7AB6}">
@@ -219,15 +228,33 @@
     </comment>
     <comment ref="N89" authorId="4" shapeId="0" xr:uid="{6386920C-1233-4144-AF76-CED9FC6768D1}">
       <text>
-        <t xml:space="preserve">Njord:
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">Njord:
 I NSR som jag kan se så är det 740? Eller 700 utan tunnfilmsmoduler?
 </t>
+        </r>
       </text>
     </comment>
     <comment ref="O89" authorId="4" shapeId="0" xr:uid="{705249D8-887B-44F9-BF41-CAC86EE06025}">
       <text>
-        <t>Njord:
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Njord:
 730 om endast modulproduktion till den inhemska marknaden ska räknas.</t>
+        </r>
       </text>
     </comment>
     <comment ref="N116" authorId="2" shapeId="0" xr:uid="{08E0E4C4-16E3-4295-85E4-6DCACE8D49C4}">
@@ -1221,9 +1248,6 @@
     <t>Togo</t>
   </si>
   <si>
-    <t>Trinidad_and_Tobago</t>
-  </si>
-  <si>
     <t>Tunisia</t>
   </si>
   <si>
@@ -1242,15 +1266,6 @@
     <t>Ukraine</t>
   </si>
   <si>
-    <t>United_Arab_Emirates</t>
-  </si>
-  <si>
-    <t>United_Kingdom</t>
-  </si>
-  <si>
-    <t>United_States_of_America</t>
-  </si>
-  <si>
     <t>Uruguay</t>
   </si>
   <si>
@@ -1260,9 +1275,6 @@
     <t>Venezuela</t>
   </si>
   <si>
-    <t>Western_Sahara</t>
-  </si>
-  <si>
     <t>Viet Nam</t>
   </si>
   <si>
@@ -1276,13 +1288,28 @@
   </si>
   <si>
     <t>Zimbabwe</t>
+  </si>
+  <si>
+    <t>United States of America</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>United Arab Emirates</t>
+  </si>
+  <si>
+    <t>Trinidad and Tobago</t>
+  </si>
+  <si>
+    <t>Western Sahara</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="19">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2319,16 +2346,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463DEAE1-12B4-4B7D-A82D-D43D3DD59FCF}">
   <dimension ref="A1:V274"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="O128" sqref="O128"/>
+    <sheetView tabSelected="1" topLeftCell="A251" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="A268" sqref="A268"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="16" max="16" width="8.85546875" customWidth="1"/>
+    <col min="16" max="16" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="15">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2396,7 +2423,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>22</v>
       </c>
@@ -2416,7 +2443,7 @@
       <c r="O2" s="9"/>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>23</v>
       </c>
@@ -2436,7 +2463,7 @@
       <c r="O3" s="9"/>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:22" ht="15">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>24</v>
       </c>
@@ -2469,7 +2496,7 @@
         <v>300.8</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="15">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>25</v>
       </c>
@@ -2497,7 +2524,7 @@
       </c>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:22">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>26</v>
       </c>
@@ -2517,7 +2544,7 @@
       <c r="O6" s="9"/>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:22">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>27</v>
       </c>
@@ -2537,7 +2564,7 @@
       <c r="O7" s="9"/>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:22">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>28</v>
       </c>
@@ -2557,7 +2584,7 @@
       <c r="O8" s="9"/>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:22">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>29</v>
       </c>
@@ -2577,7 +2604,7 @@
       <c r="O9" s="9"/>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:22">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>30</v>
       </c>
@@ -2601,7 +2628,7 @@
       <c r="O10" s="9"/>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:22">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>31</v>
       </c>
@@ -2621,7 +2648,7 @@
       <c r="O11" s="9"/>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:22">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>32</v>
       </c>
@@ -2645,7 +2672,7 @@
       <c r="O12" s="9"/>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:22">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>33</v>
       </c>
@@ -2665,7 +2692,7 @@
       <c r="O13" s="9"/>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="1:22">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>34</v>
       </c>
@@ -2707,7 +2734,7 @@
       </c>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:22">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>35</v>
       </c>
@@ -2729,7 +2756,7 @@
       <c r="O15" s="9"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:22">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
         <v>36</v>
       </c>
@@ -2759,7 +2786,7 @@
       </c>
       <c r="P16" s="1"/>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>37</v>
       </c>
@@ -2801,7 +2828,7 @@
       </c>
       <c r="P17" s="1"/>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
         <v>35</v>
       </c>
@@ -2823,7 +2850,7 @@
       <c r="O18" s="9"/>
       <c r="P18" s="1"/>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
         <v>36</v>
       </c>
@@ -2853,7 +2880,7 @@
       </c>
       <c r="P19" s="1"/>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>38</v>
       </c>
@@ -2873,7 +2900,7 @@
       <c r="O20" s="9"/>
       <c r="P20" s="1"/>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>39</v>
       </c>
@@ -2893,7 +2920,7 @@
       <c r="O21" s="9"/>
       <c r="P21" s="1"/>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>40</v>
       </c>
@@ -2913,7 +2940,7 @@
       <c r="O22" s="9"/>
       <c r="P22" s="1"/>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>41</v>
       </c>
@@ -2933,7 +2960,7 @@
       <c r="O23" s="9"/>
       <c r="P23" s="1"/>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>42</v>
       </c>
@@ -2953,7 +2980,7 @@
       <c r="O24" s="9"/>
       <c r="P24" s="1"/>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>43</v>
       </c>
@@ -2973,7 +3000,7 @@
       <c r="O25" s="9"/>
       <c r="P25" s="1"/>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>44</v>
       </c>
@@ -3005,7 +3032,7 @@
       <c r="O26" s="9"/>
       <c r="P26" s="1"/>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
         <v>36</v>
       </c>
@@ -3035,7 +3062,7 @@
       <c r="O27" s="9"/>
       <c r="P27" s="1"/>
     </row>
-    <row r="28" spans="1:16">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
         <v>32</v>
       </c>
@@ -3065,7 +3092,7 @@
       <c r="O28" s="9"/>
       <c r="P28" s="1"/>
     </row>
-    <row r="29" spans="1:16">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" s="16" t="s">
         <v>45</v>
       </c>
@@ -3095,7 +3122,7 @@
       <c r="O29" s="9"/>
       <c r="P29" s="1"/>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" s="16" t="s">
         <v>46</v>
       </c>
@@ -3121,7 +3148,7 @@
       <c r="O30" s="9"/>
       <c r="P30" s="1"/>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" s="16" t="s">
         <v>47</v>
       </c>
@@ -3145,7 +3172,7 @@
       <c r="O31" s="9"/>
       <c r="P31" s="1"/>
     </row>
-    <row r="32" spans="1:16">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" s="16" t="s">
         <v>48</v>
       </c>
@@ -3175,7 +3202,7 @@
       <c r="O32" s="9"/>
       <c r="P32" s="1"/>
     </row>
-    <row r="33" spans="1:16">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>49</v>
       </c>
@@ -3195,7 +3222,7 @@
       <c r="O33" s="9"/>
       <c r="P33" s="1"/>
     </row>
-    <row r="34" spans="1:16">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>50</v>
       </c>
@@ -3215,7 +3242,7 @@
       <c r="O34" s="9"/>
       <c r="P34" s="1"/>
     </row>
-    <row r="35" spans="1:16">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>51</v>
       </c>
@@ -3235,7 +3262,7 @@
       <c r="O35" s="9"/>
       <c r="P35" s="1"/>
     </row>
-    <row r="36" spans="1:16">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>52</v>
       </c>
@@ -3255,7 +3282,7 @@
       <c r="O36" s="9"/>
       <c r="P36" s="1"/>
     </row>
-    <row r="37" spans="1:16">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>53</v>
       </c>
@@ -3275,7 +3302,7 @@
       <c r="O37" s="9"/>
       <c r="P37" s="1"/>
     </row>
-    <row r="38" spans="1:16">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>54</v>
       </c>
@@ -3295,7 +3322,7 @@
       <c r="O38" s="9"/>
       <c r="P38" s="1"/>
     </row>
-    <row r="39" spans="1:16">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>55</v>
       </c>
@@ -3315,7 +3342,7 @@
       <c r="O39" s="9"/>
       <c r="P39" s="1"/>
     </row>
-    <row r="40" spans="1:16">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>56</v>
       </c>
@@ -3337,7 +3364,7 @@
       <c r="O40" s="9"/>
       <c r="P40" s="1"/>
     </row>
-    <row r="41" spans="1:16">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41" s="9" t="s">
         <v>31</v>
       </c>
@@ -3357,7 +3384,7 @@
       <c r="O41" s="9"/>
       <c r="P41" s="1"/>
     </row>
-    <row r="42" spans="1:16">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42" s="9" t="s">
         <v>32</v>
       </c>
@@ -3379,7 +3406,7 @@
       <c r="O42" s="9"/>
       <c r="P42" s="1"/>
     </row>
-    <row r="43" spans="1:16">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>57</v>
       </c>
@@ -3399,7 +3426,7 @@
       <c r="O43" s="9"/>
       <c r="P43" s="1"/>
     </row>
-    <row r="44" spans="1:16">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>58</v>
       </c>
@@ -3419,7 +3446,7 @@
       <c r="O44" s="9"/>
       <c r="P44" s="1"/>
     </row>
-    <row r="45" spans="1:16">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>59</v>
       </c>
@@ -3443,7 +3470,7 @@
       </c>
       <c r="P45" s="1"/>
     </row>
-    <row r="46" spans="1:16">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46" s="9" t="s">
         <v>31</v>
       </c>
@@ -3463,7 +3490,7 @@
       <c r="O46" s="9"/>
       <c r="P46" s="1"/>
     </row>
-    <row r="47" spans="1:16">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A47" s="9"/>
       <c r="B47" s="9"/>
       <c r="C47" s="9"/>
@@ -3483,7 +3510,7 @@
       </c>
       <c r="P47" s="1"/>
     </row>
-    <row r="48" spans="1:16">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>60</v>
       </c>
@@ -3503,7 +3530,7 @@
       <c r="O48" s="9"/>
       <c r="P48" s="1"/>
     </row>
-    <row r="49" spans="1:16">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>61</v>
       </c>
@@ -3523,7 +3550,7 @@
       <c r="O49" s="9"/>
       <c r="P49" s="1"/>
     </row>
-    <row r="50" spans="1:16">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>62</v>
       </c>
@@ -3543,7 +3570,7 @@
       <c r="O50" s="9"/>
       <c r="P50" s="1"/>
     </row>
-    <row r="51" spans="1:16">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>63</v>
       </c>
@@ -3586,7 +3613,7 @@
       </c>
       <c r="P51" s="1"/>
     </row>
-    <row r="52" spans="1:16">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A52" s="9" t="s">
         <v>64</v>
       </c>
@@ -3612,7 +3639,7 @@
       </c>
       <c r="P52" s="1"/>
     </row>
-    <row r="53" spans="1:16">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A53" s="9" t="s">
         <v>32</v>
       </c>
@@ -3644,7 +3671,7 @@
       <c r="O53" s="9"/>
       <c r="P53" s="1"/>
     </row>
-    <row r="54" spans="1:16">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>65</v>
       </c>
@@ -3664,7 +3691,7 @@
       <c r="O54" s="9"/>
       <c r="P54" s="1"/>
     </row>
-    <row r="55" spans="1:16">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>66</v>
       </c>
@@ -3684,7 +3711,7 @@
       <c r="O55" s="9"/>
       <c r="P55" s="1"/>
     </row>
-    <row r="56" spans="1:16">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>67</v>
       </c>
@@ -3704,7 +3731,7 @@
       <c r="O56" s="9"/>
       <c r="P56" s="1"/>
     </row>
-    <row r="57" spans="1:16">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>68</v>
       </c>
@@ -3724,7 +3751,7 @@
       <c r="O57" s="9"/>
       <c r="P57" s="1"/>
     </row>
-    <row r="58" spans="1:16">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>69</v>
       </c>
@@ -3764,7 +3791,7 @@
       </c>
       <c r="P58" s="1"/>
     </row>
-    <row r="59" spans="1:16">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A59" s="9" t="s">
         <v>64</v>
       </c>
@@ -3794,7 +3821,7 @@
       </c>
       <c r="P59" s="1"/>
     </row>
-    <row r="60" spans="1:16">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A60" s="9" t="s">
         <v>32</v>
       </c>
@@ -3826,7 +3853,7 @@
       <c r="O60" s="9"/>
       <c r="P60" s="1"/>
     </row>
-    <row r="61" spans="1:16">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>70</v>
       </c>
@@ -3846,7 +3873,7 @@
       <c r="O61" s="9"/>
       <c r="P61" s="1"/>
     </row>
-    <row r="62" spans="1:16">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>71</v>
       </c>
@@ -3866,7 +3893,7 @@
       <c r="O62" s="9"/>
       <c r="P62" s="1"/>
     </row>
-    <row r="63" spans="1:16">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>72</v>
       </c>
@@ -3886,7 +3913,7 @@
       <c r="O63" s="9"/>
       <c r="P63" s="1"/>
     </row>
-    <row r="64" spans="1:16">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>73</v>
       </c>
@@ -3906,7 +3933,7 @@
       <c r="O64" s="9"/>
       <c r="P64" s="1"/>
     </row>
-    <row r="65" spans="1:16">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>74</v>
       </c>
@@ -3926,7 +3953,7 @@
       <c r="O65" s="9"/>
       <c r="P65" s="1"/>
     </row>
-    <row r="66" spans="1:16">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>75</v>
       </c>
@@ -3946,7 +3973,7 @@
       <c r="O66" s="9"/>
       <c r="P66" s="1"/>
     </row>
-    <row r="67" spans="1:16">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>76</v>
       </c>
@@ -3966,7 +3993,7 @@
       <c r="O67" s="9"/>
       <c r="P67" s="1"/>
     </row>
-    <row r="68" spans="1:16">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>77</v>
       </c>
@@ -3986,7 +4013,7 @@
       <c r="O68" s="9"/>
       <c r="P68" s="1"/>
     </row>
-    <row r="69" spans="1:16">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>78</v>
       </c>
@@ -4006,7 +4033,7 @@
       <c r="O69" s="9"/>
       <c r="P69" s="1"/>
     </row>
-    <row r="70" spans="1:16">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>79</v>
       </c>
@@ -4026,7 +4053,7 @@
       <c r="O70" s="9"/>
       <c r="P70" s="1"/>
     </row>
-    <row r="71" spans="1:16">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>80</v>
       </c>
@@ -4058,7 +4085,7 @@
       <c r="O71" s="9"/>
       <c r="P71" s="1"/>
     </row>
-    <row r="72" spans="1:16">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A72" s="9" t="s">
         <v>64</v>
       </c>
@@ -4082,7 +4109,7 @@
       <c r="O72" s="9"/>
       <c r="P72" s="1"/>
     </row>
-    <row r="73" spans="1:16">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A73" s="9" t="s">
         <v>32</v>
       </c>
@@ -4104,7 +4131,7 @@
       <c r="O73" s="9"/>
       <c r="P73" s="1"/>
     </row>
-    <row r="74" spans="1:16">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>81</v>
       </c>
@@ -4124,7 +4151,7 @@
       <c r="O74" s="9"/>
       <c r="P74" s="1"/>
     </row>
-    <row r="75" spans="1:16">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>82</v>
       </c>
@@ -4144,7 +4171,7 @@
       <c r="O75" s="9"/>
       <c r="P75" s="1"/>
     </row>
-    <row r="76" spans="1:16">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>83</v>
       </c>
@@ -4164,7 +4191,7 @@
       <c r="O76" s="9"/>
       <c r="P76" s="1"/>
     </row>
-    <row r="77" spans="1:16">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>84</v>
       </c>
@@ -4184,7 +4211,7 @@
       <c r="O77" s="9"/>
       <c r="P77" s="1"/>
     </row>
-    <row r="78" spans="1:16">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>85</v>
       </c>
@@ -4208,7 +4235,7 @@
       <c r="O78" s="9"/>
       <c r="P78" s="1"/>
     </row>
-    <row r="79" spans="1:16">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A79" s="14" t="s">
         <v>86</v>
       </c>
@@ -4232,7 +4259,7 @@
       <c r="O79" s="9"/>
       <c r="P79" s="1"/>
     </row>
-    <row r="80" spans="1:16">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>87</v>
       </c>
@@ -4252,7 +4279,7 @@
       <c r="O80" s="9"/>
       <c r="P80" s="1"/>
     </row>
-    <row r="81" spans="1:16">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>88</v>
       </c>
@@ -4272,7 +4299,7 @@
       <c r="O81" s="9"/>
       <c r="P81" s="1"/>
     </row>
-    <row r="82" spans="1:16">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>89</v>
       </c>
@@ -4292,7 +4319,7 @@
       <c r="O82" s="9"/>
       <c r="P82" s="1"/>
     </row>
-    <row r="83" spans="1:16">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>90</v>
       </c>
@@ -4312,7 +4339,7 @@
       <c r="O83" s="9"/>
       <c r="P83" s="1"/>
     </row>
-    <row r="84" spans="1:16">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>91</v>
       </c>
@@ -4332,7 +4359,7 @@
       <c r="O84" s="9"/>
       <c r="P84" s="1"/>
     </row>
-    <row r="85" spans="1:16">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>92</v>
       </c>
@@ -4352,7 +4379,7 @@
       <c r="O85" s="9"/>
       <c r="P85" s="1"/>
     </row>
-    <row r="86" spans="1:16">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>93</v>
       </c>
@@ -4384,7 +4411,7 @@
       <c r="O86" s="9"/>
       <c r="P86" s="1"/>
     </row>
-    <row r="87" spans="1:16">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A87" s="9" t="s">
         <v>64</v>
       </c>
@@ -4416,7 +4443,7 @@
       <c r="O87" s="9"/>
       <c r="P87" s="1"/>
     </row>
-    <row r="88" spans="1:16">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>95</v>
       </c>
@@ -4441,10 +4468,12 @@
       <c r="N88" s="8">
         <v>300</v>
       </c>
-      <c r="O88" s="9"/>
+      <c r="O88" s="9">
+        <v>840</v>
+      </c>
       <c r="P88" s="1"/>
     </row>
-    <row r="89" spans="1:16" ht="15">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A89" s="9" t="s">
         <v>64</v>
       </c>
@@ -4472,7 +4501,7 @@
       </c>
       <c r="P89" s="1"/>
     </row>
-    <row r="90" spans="1:16" ht="15">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A90" s="9" t="s">
         <v>32</v>
       </c>
@@ -4500,7 +4529,7 @@
       <c r="O90" s="9"/>
       <c r="P90" s="1"/>
     </row>
-    <row r="91" spans="1:16">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>96</v>
       </c>
@@ -4520,7 +4549,7 @@
       <c r="O91" s="9"/>
       <c r="P91" s="1"/>
     </row>
-    <row r="92" spans="1:16">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>97</v>
       </c>
@@ -4540,7 +4569,7 @@
       <c r="O92" s="9"/>
       <c r="P92" s="1"/>
     </row>
-    <row r="93" spans="1:16">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>98</v>
       </c>
@@ -4560,7 +4589,7 @@
       <c r="O93" s="9"/>
       <c r="P93" s="1"/>
     </row>
-    <row r="94" spans="1:16">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>99</v>
       </c>
@@ -4580,7 +4609,7 @@
       <c r="O94" s="9"/>
       <c r="P94" s="1"/>
     </row>
-    <row r="95" spans="1:16">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>100</v>
       </c>
@@ -4620,7 +4649,7 @@
       <c r="O95" s="20"/>
       <c r="P95" s="1"/>
     </row>
-    <row r="96" spans="1:16">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A96" s="9" t="s">
         <v>64</v>
       </c>
@@ -4644,7 +4673,7 @@
       <c r="O96" s="9"/>
       <c r="P96" s="1"/>
     </row>
-    <row r="97" spans="1:16">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A97" s="9" t="s">
         <v>32</v>
       </c>
@@ -4672,7 +4701,7 @@
       <c r="O97" s="9"/>
       <c r="P97" s="1"/>
     </row>
-    <row r="98" spans="1:16">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>101</v>
       </c>
@@ -4700,7 +4729,7 @@
       <c r="O98" s="9"/>
       <c r="P98" s="1"/>
     </row>
-    <row r="99" spans="1:16">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A99" s="14" t="s">
         <v>102</v>
       </c>
@@ -4728,7 +4757,7 @@
       <c r="O99" s="9"/>
       <c r="P99" s="1"/>
     </row>
-    <row r="100" spans="1:16">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>103</v>
       </c>
@@ -4748,7 +4777,7 @@
       <c r="O100" s="9"/>
       <c r="P100" s="1"/>
     </row>
-    <row r="101" spans="1:16">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>104</v>
       </c>
@@ -4768,7 +4797,7 @@
       <c r="O101" s="9"/>
       <c r="P101" s="1"/>
     </row>
-    <row r="102" spans="1:16">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>105</v>
       </c>
@@ -4788,7 +4817,7 @@
       <c r="O102" s="9"/>
       <c r="P102" s="1"/>
     </row>
-    <row r="103" spans="1:16">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>106</v>
       </c>
@@ -4808,7 +4837,7 @@
       <c r="O103" s="9"/>
       <c r="P103" s="1"/>
     </row>
-    <row r="104" spans="1:16">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
         <v>107</v>
       </c>
@@ -4828,7 +4857,7 @@
       <c r="O104" s="9"/>
       <c r="P104" s="1"/>
     </row>
-    <row r="105" spans="1:16">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
         <v>108</v>
       </c>
@@ -4848,7 +4877,7 @@
       <c r="O105" s="9"/>
       <c r="P105" s="1"/>
     </row>
-    <row r="106" spans="1:16">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>109</v>
       </c>
@@ -4868,7 +4897,7 @@
       <c r="O106" s="9"/>
       <c r="P106" s="1"/>
     </row>
-    <row r="107" spans="1:16">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
         <v>110</v>
       </c>
@@ -4888,7 +4917,7 @@
       <c r="O107" s="9"/>
       <c r="P107" s="1"/>
     </row>
-    <row r="108" spans="1:16">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
         <v>111</v>
       </c>
@@ -4908,7 +4937,7 @@
       <c r="O108" s="9"/>
       <c r="P108" s="1"/>
     </row>
-    <row r="109" spans="1:16">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
         <v>112</v>
       </c>
@@ -4928,7 +4957,7 @@
       <c r="O109" s="9"/>
       <c r="P109" s="1"/>
     </row>
-    <row r="110" spans="1:16">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
         <v>113</v>
       </c>
@@ -4948,7 +4977,7 @@
       <c r="O110" s="9"/>
       <c r="P110" s="1"/>
     </row>
-    <row r="111" spans="1:16">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>114</v>
       </c>
@@ -4968,7 +4997,7 @@
       <c r="O111" s="9"/>
       <c r="P111" s="1"/>
     </row>
-    <row r="112" spans="1:16">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
         <v>115</v>
       </c>
@@ -4988,7 +5017,7 @@
       <c r="O112" s="9"/>
       <c r="P112" s="1"/>
     </row>
-    <row r="113" spans="1:16">
+    <row r="113" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>116</v>
       </c>
@@ -5008,7 +5037,7 @@
       <c r="O113" s="9"/>
       <c r="P113" s="1"/>
     </row>
-    <row r="114" spans="1:16">
+    <row r="114" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
         <v>117</v>
       </c>
@@ -5038,7 +5067,7 @@
       </c>
       <c r="P114" s="1"/>
     </row>
-    <row r="115" spans="1:16">
+    <row r="115" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A115" s="24" t="s">
         <v>32</v>
       </c>
@@ -5066,7 +5095,7 @@
       <c r="O115" s="24"/>
       <c r="P115" s="24"/>
     </row>
-    <row r="116" spans="1:16">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>118</v>
       </c>
@@ -5086,7 +5115,7 @@
       <c r="O116" s="9"/>
       <c r="P116" s="1"/>
     </row>
-    <row r="117" spans="1:16">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
         <v>119</v>
       </c>
@@ -5106,7 +5135,7 @@
       <c r="O117" s="9"/>
       <c r="P117" s="1"/>
     </row>
-    <row r="118" spans="1:16">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
         <v>120</v>
       </c>
@@ -5126,7 +5155,7 @@
       <c r="O118" s="9"/>
       <c r="P118" s="1"/>
     </row>
-    <row r="119" spans="1:16">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
         <v>121</v>
       </c>
@@ -5146,7 +5175,7 @@
       <c r="O119" s="9"/>
       <c r="P119" s="1"/>
     </row>
-    <row r="120" spans="1:16">
+    <row r="120" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
         <v>122</v>
       </c>
@@ -5166,7 +5195,7 @@
       <c r="O120" s="9"/>
       <c r="P120" s="1"/>
     </row>
-    <row r="121" spans="1:16">
+    <row r="121" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
         <v>123</v>
       </c>
@@ -5192,7 +5221,7 @@
         <v>140</v>
       </c>
       <c r="L121" s="6">
-        <v>0</v>
+        <v>63.3</v>
       </c>
       <c r="M121" s="7">
         <v>190</v>
@@ -5205,7 +5234,7 @@
       </c>
       <c r="P121" s="1"/>
     </row>
-    <row r="122" spans="1:16">
+    <row r="122" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A122" s="9" t="s">
         <v>64</v>
       </c>
@@ -5223,7 +5252,9 @@
         <v>215</v>
       </c>
       <c r="K122" s="9"/>
-      <c r="L122" s="9"/>
+      <c r="L122" s="9">
+        <v>63.3</v>
+      </c>
       <c r="M122" s="9"/>
       <c r="N122" s="9">
         <v>48.74</v>
@@ -5233,7 +5264,7 @@
       </c>
       <c r="P122" s="1"/>
     </row>
-    <row r="123" spans="1:16">
+    <row r="123" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A123" s="9" t="s">
         <v>32</v>
       </c>
@@ -5257,7 +5288,7 @@
       <c r="O123" s="9"/>
       <c r="P123" s="1"/>
     </row>
-    <row r="124" spans="1:16">
+    <row r="124" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
         <v>124</v>
       </c>
@@ -5277,7 +5308,7 @@
       <c r="O124" s="9"/>
       <c r="P124" s="1"/>
     </row>
-    <row r="125" spans="1:16">
+    <row r="125" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
         <v>125</v>
       </c>
@@ -5297,7 +5328,7 @@
       <c r="O125" s="9"/>
       <c r="P125" s="1"/>
     </row>
-    <row r="126" spans="1:16">
+    <row r="126" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
         <v>126</v>
       </c>
@@ -5340,7 +5371,7 @@
       </c>
       <c r="P126" s="1"/>
     </row>
-    <row r="127" spans="1:16">
+    <row r="127" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A127" s="9" t="s">
         <v>64</v>
       </c>
@@ -5375,7 +5406,7 @@
       </c>
       <c r="P127" s="1"/>
     </row>
-    <row r="128" spans="1:16">
+    <row r="128" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A128" s="9" t="s">
         <v>32</v>
       </c>
@@ -5407,7 +5438,7 @@
       <c r="O128" s="9"/>
       <c r="P128" s="1"/>
     </row>
-    <row r="129" spans="1:16">
+    <row r="129" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
         <v>127</v>
       </c>
@@ -5427,7 +5458,7 @@
       <c r="O129" s="9"/>
       <c r="P129" s="1"/>
     </row>
-    <row r="130" spans="1:16">
+    <row r="130" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
         <v>128</v>
       </c>
@@ -5447,7 +5478,7 @@
       <c r="O130" s="9"/>
       <c r="P130" s="1"/>
     </row>
-    <row r="131" spans="1:16">
+    <row r="131" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
         <v>129</v>
       </c>
@@ -5467,7 +5498,7 @@
       <c r="O131" s="9"/>
       <c r="P131" s="1"/>
     </row>
-    <row r="132" spans="1:16">
+    <row r="132" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
         <v>130</v>
       </c>
@@ -5487,7 +5518,7 @@
       <c r="O132" s="9"/>
       <c r="P132" s="1"/>
     </row>
-    <row r="133" spans="1:16">
+    <row r="133" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
         <v>131</v>
       </c>
@@ -5507,7 +5538,7 @@
       <c r="O133" s="9"/>
       <c r="P133" s="1"/>
     </row>
-    <row r="134" spans="1:16">
+    <row r="134" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
         <v>132</v>
       </c>
@@ -5527,7 +5558,7 @@
       <c r="O134" s="9"/>
       <c r="P134" s="1"/>
     </row>
-    <row r="135" spans="1:16">
+    <row r="135" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
         <v>133</v>
       </c>
@@ -5547,7 +5578,7 @@
       <c r="O135" s="9"/>
       <c r="P135" s="1"/>
     </row>
-    <row r="136" spans="1:16">
+    <row r="136" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
         <v>134</v>
       </c>
@@ -5567,7 +5598,7 @@
       <c r="O136" s="9"/>
       <c r="P136" s="1"/>
     </row>
-    <row r="137" spans="1:16">
+    <row r="137" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
         <v>135</v>
       </c>
@@ -5587,7 +5618,7 @@
       <c r="O137" s="9"/>
       <c r="P137" s="1"/>
     </row>
-    <row r="138" spans="1:16">
+    <row r="138" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
         <v>136</v>
       </c>
@@ -5607,7 +5638,7 @@
       <c r="O138" s="9"/>
       <c r="P138" s="1"/>
     </row>
-    <row r="139" spans="1:16">
+    <row r="139" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
         <v>137</v>
       </c>
@@ -5627,7 +5658,7 @@
       <c r="O139" s="9"/>
       <c r="P139" s="1"/>
     </row>
-    <row r="140" spans="1:16">
+    <row r="140" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
         <v>138</v>
       </c>
@@ -5647,7 +5678,7 @@
       <c r="O140" s="9"/>
       <c r="P140" s="1"/>
     </row>
-    <row r="141" spans="1:16">
+    <row r="141" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
         <v>139</v>
       </c>
@@ -5667,7 +5698,7 @@
       <c r="O141" s="9"/>
       <c r="P141" s="1"/>
     </row>
-    <row r="142" spans="1:16">
+    <row r="142" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
         <v>140</v>
       </c>
@@ -5687,7 +5718,7 @@
       <c r="O142" s="9"/>
       <c r="P142" s="1"/>
     </row>
-    <row r="143" spans="1:16">
+    <row r="143" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
         <v>141</v>
       </c>
@@ -5707,7 +5738,7 @@
       <c r="O143" s="9"/>
       <c r="P143" s="1"/>
     </row>
-    <row r="144" spans="1:16">
+    <row r="144" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
         <v>142</v>
       </c>
@@ -5727,7 +5758,7 @@
       <c r="O144" s="9"/>
       <c r="P144" s="1"/>
     </row>
-    <row r="145" spans="1:16">
+    <row r="145" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
         <v>143</v>
       </c>
@@ -5747,7 +5778,7 @@
       <c r="O145" s="9"/>
       <c r="P145" s="1"/>
     </row>
-    <row r="146" spans="1:16">
+    <row r="146" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
         <v>144</v>
       </c>
@@ -5767,7 +5798,7 @@
       <c r="O146" s="9"/>
       <c r="P146" s="1"/>
     </row>
-    <row r="147" spans="1:16">
+    <row r="147" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A147" s="2" t="s">
         <v>145</v>
       </c>
@@ -5797,7 +5828,7 @@
       </c>
       <c r="P147" s="1"/>
     </row>
-    <row r="148" spans="1:16">
+    <row r="148" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A148" s="9" t="s">
         <v>64</v>
       </c>
@@ -5829,7 +5860,7 @@
       <c r="O148" s="9"/>
       <c r="P148" s="1"/>
     </row>
-    <row r="149" spans="1:16">
+    <row r="149" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A149" s="9" t="s">
         <v>32</v>
       </c>
@@ -5855,7 +5886,7 @@
       <c r="O149" s="9"/>
       <c r="P149" s="1"/>
     </row>
-    <row r="150" spans="1:16">
+    <row r="150" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A150" s="2" t="s">
         <v>146</v>
       </c>
@@ -5875,7 +5906,7 @@
       <c r="O150" s="9"/>
       <c r="P150" s="1"/>
     </row>
-    <row r="151" spans="1:16">
+    <row r="151" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A151" s="2" t="s">
         <v>147</v>
       </c>
@@ -5895,7 +5926,7 @@
       <c r="O151" s="9"/>
       <c r="P151" s="1"/>
     </row>
-    <row r="152" spans="1:16">
+    <row r="152" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A152" s="2" t="s">
         <v>148</v>
       </c>
@@ -5915,7 +5946,7 @@
       <c r="O152" s="9"/>
       <c r="P152" s="1"/>
     </row>
-    <row r="153" spans="1:16">
+    <row r="153" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A153" s="2" t="s">
         <v>149</v>
       </c>
@@ -5935,7 +5966,7 @@
       <c r="O153" s="9"/>
       <c r="P153" s="1"/>
     </row>
-    <row r="154" spans="1:16">
+    <row r="154" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A154" s="2" t="s">
         <v>150</v>
       </c>
@@ -5955,7 +5986,7 @@
       <c r="O154" s="9"/>
       <c r="P154" s="1"/>
     </row>
-    <row r="155" spans="1:16">
+    <row r="155" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A155" s="2" t="s">
         <v>151</v>
       </c>
@@ -5975,7 +6006,7 @@
       <c r="O155" s="9"/>
       <c r="P155" s="1"/>
     </row>
-    <row r="156" spans="1:16">
+    <row r="156" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A156" s="2" t="s">
         <v>152</v>
       </c>
@@ -6005,7 +6036,7 @@
       <c r="O156" s="9"/>
       <c r="P156" s="1"/>
     </row>
-    <row r="157" spans="1:16">
+    <row r="157" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A157" s="9" t="s">
         <v>64</v>
       </c>
@@ -6029,7 +6060,7 @@
       <c r="O157" s="9"/>
       <c r="P157" s="1"/>
     </row>
-    <row r="158" spans="1:16">
+    <row r="158" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A158" s="9" t="s">
         <v>32</v>
       </c>
@@ -6059,7 +6090,7 @@
       <c r="O158" s="9"/>
       <c r="P158" s="1"/>
     </row>
-    <row r="159" spans="1:16">
+    <row r="159" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A159" s="2" t="s">
         <v>153</v>
       </c>
@@ -6079,7 +6110,7 @@
       <c r="O159" s="9"/>
       <c r="P159" s="1"/>
     </row>
-    <row r="160" spans="1:16">
+    <row r="160" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A160" s="2" t="s">
         <v>154</v>
       </c>
@@ -6099,7 +6130,7 @@
       <c r="O160" s="9"/>
       <c r="P160" s="1"/>
     </row>
-    <row r="161" spans="1:16">
+    <row r="161" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A161" s="2" t="s">
         <v>155</v>
       </c>
@@ -6119,7 +6150,7 @@
       <c r="O161" s="9"/>
       <c r="P161" s="1"/>
     </row>
-    <row r="162" spans="1:16">
+    <row r="162" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A162" s="2" t="s">
         <v>156</v>
       </c>
@@ -6141,7 +6172,7 @@
       <c r="O162" s="9"/>
       <c r="P162" s="1"/>
     </row>
-    <row r="163" spans="1:16">
+    <row r="163" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A163" s="9" t="s">
         <v>25</v>
       </c>
@@ -6163,7 +6194,7 @@
       <c r="O163" s="25"/>
       <c r="P163" s="1"/>
     </row>
-    <row r="164" spans="1:16">
+    <row r="164" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A164" s="2" t="s">
         <v>157</v>
       </c>
@@ -6183,7 +6214,7 @@
       <c r="O164" s="9"/>
       <c r="P164" s="1"/>
     </row>
-    <row r="165" spans="1:16">
+    <row r="165" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A165" s="2" t="s">
         <v>158</v>
       </c>
@@ -6203,7 +6234,7 @@
       <c r="O165" s="9"/>
       <c r="P165" s="1"/>
     </row>
-    <row r="166" spans="1:16">
+    <row r="166" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A166" s="2" t="s">
         <v>159</v>
       </c>
@@ -6223,7 +6254,7 @@
       <c r="O166" s="9"/>
       <c r="P166" s="1"/>
     </row>
-    <row r="167" spans="1:16">
+    <row r="167" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A167" s="2" t="s">
         <v>160</v>
       </c>
@@ -6243,7 +6274,7 @@
       <c r="O167" s="9"/>
       <c r="P167" s="1"/>
     </row>
-    <row r="168" spans="1:16">
+    <row r="168" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A168" s="2" t="s">
         <v>161</v>
       </c>
@@ -6271,7 +6302,7 @@
       <c r="O168" s="9"/>
       <c r="P168" s="1"/>
     </row>
-    <row r="169" spans="1:16">
+    <row r="169" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A169" s="9" t="s">
         <v>32</v>
       </c>
@@ -6295,7 +6326,7 @@
       <c r="O169" s="9"/>
       <c r="P169" s="1"/>
     </row>
-    <row r="170" spans="1:16">
+    <row r="170" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A170" s="2" t="s">
         <v>162</v>
       </c>
@@ -6315,7 +6346,7 @@
       <c r="O170" s="9"/>
       <c r="P170" s="1"/>
     </row>
-    <row r="171" spans="1:16">
+    <row r="171" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A171" s="2" t="s">
         <v>163</v>
       </c>
@@ -6335,7 +6366,7 @@
       <c r="O171" s="9"/>
       <c r="P171" s="1"/>
     </row>
-    <row r="172" spans="1:16">
+    <row r="172" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A172" s="2" t="s">
         <v>164</v>
       </c>
@@ -6355,7 +6386,7 @@
       <c r="O172" s="9"/>
       <c r="P172" s="1"/>
     </row>
-    <row r="173" spans="1:16">
+    <row r="173" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A173" s="2" t="s">
         <v>165</v>
       </c>
@@ -6375,7 +6406,7 @@
       <c r="O173" s="9"/>
       <c r="P173" s="1"/>
     </row>
-    <row r="174" spans="1:16">
+    <row r="174" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A174" s="2" t="s">
         <v>166</v>
       </c>
@@ -6395,7 +6426,7 @@
       <c r="O174" s="9"/>
       <c r="P174" s="1"/>
     </row>
-    <row r="175" spans="1:16">
+    <row r="175" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A175" s="2" t="s">
         <v>167</v>
       </c>
@@ -6415,7 +6446,7 @@
       <c r="O175" s="9"/>
       <c r="P175" s="1"/>
     </row>
-    <row r="176" spans="1:16">
+    <row r="176" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A176" s="2" t="s">
         <v>168</v>
       </c>
@@ -6435,7 +6466,7 @@
       <c r="O176" s="9"/>
       <c r="P176" s="1"/>
     </row>
-    <row r="177" spans="1:16">
+    <row r="177" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A177" s="2" t="s">
         <v>169</v>
       </c>
@@ -6455,7 +6486,7 @@
       <c r="O177" s="9"/>
       <c r="P177" s="1"/>
     </row>
-    <row r="178" spans="1:16">
+    <row r="178" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A178" s="2" t="s">
         <v>170</v>
       </c>
@@ -6475,7 +6506,7 @@
       <c r="O178" s="9"/>
       <c r="P178" s="1"/>
     </row>
-    <row r="179" spans="1:16">
+    <row r="179" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A179" s="2" t="s">
         <v>171</v>
       </c>
@@ -6495,7 +6526,7 @@
       <c r="O179" s="9"/>
       <c r="P179" s="1"/>
     </row>
-    <row r="180" spans="1:16">
+    <row r="180" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A180" s="2" t="s">
         <v>172</v>
       </c>
@@ -6515,7 +6546,7 @@
       <c r="O180" s="9"/>
       <c r="P180" s="1"/>
     </row>
-    <row r="181" spans="1:16">
+    <row r="181" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A181" s="2" t="s">
         <v>173</v>
       </c>
@@ -6535,7 +6566,7 @@
       <c r="O181" s="9"/>
       <c r="P181" s="1"/>
     </row>
-    <row r="182" spans="1:16">
+    <row r="182" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A182" s="2" t="s">
         <v>174</v>
       </c>
@@ -6555,7 +6586,7 @@
       <c r="O182" s="9"/>
       <c r="P182" s="1"/>
     </row>
-    <row r="183" spans="1:16">
+    <row r="183" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A183" s="2" t="s">
         <v>175</v>
       </c>
@@ -6575,7 +6606,7 @@
       <c r="O183" s="9"/>
       <c r="P183" s="1"/>
     </row>
-    <row r="184" spans="1:16">
+    <row r="184" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A184" s="2" t="s">
         <v>176</v>
       </c>
@@ -6595,7 +6626,7 @@
       <c r="O184" s="9"/>
       <c r="P184" s="1"/>
     </row>
-    <row r="185" spans="1:16">
+    <row r="185" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A185" s="2" t="s">
         <v>177</v>
       </c>
@@ -6615,7 +6646,7 @@
       <c r="O185" s="9"/>
       <c r="P185" s="1"/>
     </row>
-    <row r="186" spans="1:16">
+    <row r="186" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A186" s="2" t="s">
         <v>178</v>
       </c>
@@ -6643,7 +6674,7 @@
       <c r="O186" s="9"/>
       <c r="P186" s="1"/>
     </row>
-    <row r="187" spans="1:16">
+    <row r="187" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A187" s="9" t="s">
         <v>64</v>
       </c>
@@ -6665,7 +6696,7 @@
       <c r="O187" s="9"/>
       <c r="P187" s="1"/>
     </row>
-    <row r="188" spans="1:16">
+    <row r="188" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A188" s="9" t="s">
         <v>32</v>
       </c>
@@ -6689,7 +6720,7 @@
       <c r="O188" s="9"/>
       <c r="P188" s="1"/>
     </row>
-    <row r="189" spans="1:16">
+    <row r="189" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A189" s="2" t="s">
         <v>179</v>
       </c>
@@ -6709,7 +6740,7 @@
       <c r="O189" s="9"/>
       <c r="P189" s="1"/>
     </row>
-    <row r="190" spans="1:16">
+    <row r="190" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A190" s="2" t="s">
         <v>180</v>
       </c>
@@ -6735,7 +6766,7 @@
       <c r="O190" s="9"/>
       <c r="P190" s="1"/>
     </row>
-    <row r="191" spans="1:16">
+    <row r="191" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A191" s="9" t="s">
         <v>64</v>
       </c>
@@ -6759,7 +6790,7 @@
       <c r="O191" s="9"/>
       <c r="P191" s="1"/>
     </row>
-    <row r="192" spans="1:16">
+    <row r="192" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A192" s="9" t="s">
         <v>32</v>
       </c>
@@ -6781,7 +6812,7 @@
       <c r="O192" s="9"/>
       <c r="P192" s="1"/>
     </row>
-    <row r="193" spans="1:16">
+    <row r="193" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A193" s="2" t="s">
         <v>181</v>
       </c>
@@ -6801,7 +6832,7 @@
       <c r="O193" s="9"/>
       <c r="P193" s="1"/>
     </row>
-    <row r="194" spans="1:16">
+    <row r="194" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A194" s="2" t="s">
         <v>182</v>
       </c>
@@ -6833,7 +6864,7 @@
       <c r="O194" s="9"/>
       <c r="P194" s="1"/>
     </row>
-    <row r="195" spans="1:16">
+    <row r="195" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A195" s="14" t="s">
         <v>25</v>
       </c>
@@ -6865,7 +6896,7 @@
       <c r="O195" s="9"/>
       <c r="P195" s="1"/>
     </row>
-    <row r="196" spans="1:16">
+    <row r="196" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A196" s="2" t="s">
         <v>183</v>
       </c>
@@ -6885,7 +6916,7 @@
       <c r="O196" s="9"/>
       <c r="P196" s="1"/>
     </row>
-    <row r="197" spans="1:16">
+    <row r="197" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A197" s="2" t="s">
         <v>184</v>
       </c>
@@ -6905,7 +6936,7 @@
       <c r="O197" s="9"/>
       <c r="P197" s="1"/>
     </row>
-    <row r="198" spans="1:16">
+    <row r="198" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A198" s="2" t="s">
         <v>185</v>
       </c>
@@ -6927,7 +6958,7 @@
       <c r="O198" s="9"/>
       <c r="P198" s="1"/>
     </row>
-    <row r="199" spans="1:16">
+    <row r="199" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A199" s="9" t="s">
         <v>32</v>
       </c>
@@ -6949,7 +6980,7 @@
       <c r="O199" s="9"/>
       <c r="P199" s="1"/>
     </row>
-    <row r="200" spans="1:16">
+    <row r="200" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A200" s="2" t="s">
         <v>186</v>
       </c>
@@ -6969,7 +7000,7 @@
       <c r="O200" s="9"/>
       <c r="P200" s="1"/>
     </row>
-    <row r="201" spans="1:16">
+    <row r="201" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A201" s="2" t="s">
         <v>187</v>
       </c>
@@ -6989,7 +7020,7 @@
       <c r="O201" s="9"/>
       <c r="P201" s="1"/>
     </row>
-    <row r="202" spans="1:16">
+    <row r="202" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A202" s="2" t="s">
         <v>188</v>
       </c>
@@ -7009,7 +7040,7 @@
       <c r="O202" s="9"/>
       <c r="P202" s="1"/>
     </row>
-    <row r="203" spans="1:16">
+    <row r="203" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A203" s="2" t="s">
         <v>189</v>
       </c>
@@ -7029,7 +7060,7 @@
       <c r="O203" s="9"/>
       <c r="P203" s="1"/>
     </row>
-    <row r="204" spans="1:16">
+    <row r="204" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A204" s="2" t="s">
         <v>190</v>
       </c>
@@ -7049,7 +7080,7 @@
       <c r="O204" s="9"/>
       <c r="P204" s="1"/>
     </row>
-    <row r="205" spans="1:16">
+    <row r="205" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A205" s="2" t="s">
         <v>191</v>
       </c>
@@ -7085,7 +7116,7 @@
         <v>524.79999999999995</v>
       </c>
     </row>
-    <row r="206" spans="1:16">
+    <row r="206" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A206" s="29" t="s">
         <v>192</v>
       </c>
@@ -7105,7 +7136,7 @@
       <c r="O206" s="9"/>
       <c r="P206" s="30"/>
     </row>
-    <row r="207" spans="1:16">
+    <row r="207" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A207" s="29" t="s">
         <v>193</v>
       </c>
@@ -7127,7 +7158,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="208" spans="1:16" ht="240">
+    <row r="208" spans="1:16" ht="240" x14ac:dyDescent="0.3">
       <c r="A208" s="31" t="s">
         <v>194</v>
       </c>
@@ -7163,7 +7194,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="209" spans="1:16" ht="36">
+    <row r="209" spans="1:16" ht="36" x14ac:dyDescent="0.3">
       <c r="A209" s="32" t="s">
         <v>195</v>
       </c>
@@ -7191,7 +7222,7 @@
         <v>76.8</v>
       </c>
     </row>
-    <row r="210" spans="1:16" ht="24">
+    <row r="210" spans="1:16" ht="24" x14ac:dyDescent="0.3">
       <c r="A210" s="32" t="s">
         <v>196</v>
       </c>
@@ -7225,7 +7256,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="211" spans="1:16" ht="36">
+    <row r="211" spans="1:16" ht="36" x14ac:dyDescent="0.3">
       <c r="A211" s="32" t="s">
         <v>197</v>
       </c>
@@ -7245,7 +7276,7 @@
       <c r="O211" s="9"/>
       <c r="P211" s="25"/>
     </row>
-    <row r="212" spans="1:16">
+    <row r="212" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A212" s="2" t="s">
         <v>198</v>
       </c>
@@ -7265,7 +7296,7 @@
       <c r="O212" s="9"/>
       <c r="P212" s="1"/>
     </row>
-    <row r="213" spans="1:16">
+    <row r="213" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A213" s="2" t="s">
         <v>199</v>
       </c>
@@ -7285,7 +7316,7 @@
       <c r="O213" s="9"/>
       <c r="P213" s="1"/>
     </row>
-    <row r="214" spans="1:16">
+    <row r="214" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A214" s="2" t="s">
         <v>200</v>
       </c>
@@ -7305,7 +7336,7 @@
       <c r="O214" s="9"/>
       <c r="P214" s="1"/>
     </row>
-    <row r="215" spans="1:16">
+    <row r="215" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A215" s="2" t="s">
         <v>201</v>
       </c>
@@ -7325,7 +7356,7 @@
       <c r="O215" s="9"/>
       <c r="P215" s="1"/>
     </row>
-    <row r="216" spans="1:16">
+    <row r="216" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A216" s="2" t="s">
         <v>202</v>
       </c>
@@ -7361,7 +7392,7 @@
       </c>
       <c r="P216" s="1"/>
     </row>
-    <row r="217" spans="1:16">
+    <row r="217" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A217" s="9" t="s">
         <v>203</v>
       </c>
@@ -7391,7 +7422,7 @@
       <c r="O217" s="9"/>
       <c r="P217" s="1"/>
     </row>
-    <row r="218" spans="1:16">
+    <row r="218" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A218" s="9" t="s">
         <v>204</v>
       </c>
@@ -7421,7 +7452,7 @@
       <c r="O218" s="9"/>
       <c r="P218" s="1"/>
     </row>
-    <row r="219" spans="1:16">
+    <row r="219" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A219" s="2" t="s">
         <v>205</v>
       </c>
@@ -7441,7 +7472,7 @@
       <c r="O219" s="9"/>
       <c r="P219" s="1"/>
     </row>
-    <row r="220" spans="1:16">
+    <row r="220" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A220" s="2" t="s">
         <v>206</v>
       </c>
@@ -7463,7 +7494,7 @@
       <c r="O220" s="9"/>
       <c r="P220" s="1"/>
     </row>
-    <row r="221" spans="1:16">
+    <row r="221" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A221" s="9" t="s">
         <v>32</v>
       </c>
@@ -7485,7 +7516,7 @@
       <c r="O221" s="9"/>
       <c r="P221" s="1"/>
     </row>
-    <row r="222" spans="1:16">
+    <row r="222" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A222" s="2" t="s">
         <v>207</v>
       </c>
@@ -7505,7 +7536,7 @@
       <c r="O222" s="9"/>
       <c r="P222" s="1"/>
     </row>
-    <row r="223" spans="1:16">
+    <row r="223" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A223" s="2" t="s">
         <v>208</v>
       </c>
@@ -7525,7 +7556,7 @@
       <c r="O223" s="9"/>
       <c r="P223" s="1"/>
     </row>
-    <row r="224" spans="1:16">
+    <row r="224" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A224" s="2" t="s">
         <v>209</v>
       </c>
@@ -7553,7 +7584,7 @@
       <c r="O224" s="9"/>
       <c r="P224" s="1"/>
     </row>
-    <row r="225" spans="1:16">
+    <row r="225" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A225" s="16" t="s">
         <v>210</v>
       </c>
@@ -7581,7 +7612,7 @@
       <c r="O225" s="16"/>
       <c r="P225" s="1"/>
     </row>
-    <row r="226" spans="1:16">
+    <row r="226" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A226" s="2" t="s">
         <v>211</v>
       </c>
@@ -7624,7 +7655,7 @@
       </c>
       <c r="P226" s="1"/>
     </row>
-    <row r="227" spans="1:16">
+    <row r="227" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A227" s="9" t="s">
         <v>64</v>
       </c>
@@ -7656,7 +7687,7 @@
       <c r="O227" s="9"/>
       <c r="P227" s="1"/>
     </row>
-    <row r="228" spans="1:16">
+    <row r="228" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A228" s="9" t="s">
         <v>32</v>
       </c>
@@ -7682,7 +7713,7 @@
       <c r="O228" s="9"/>
       <c r="P228" s="1"/>
     </row>
-    <row r="229" spans="1:16">
+    <row r="229" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A229" s="2" t="s">
         <v>212</v>
       </c>
@@ -7702,7 +7733,7 @@
       <c r="O229" s="9"/>
       <c r="P229" s="1"/>
     </row>
-    <row r="230" spans="1:16">
+    <row r="230" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A230" s="2" t="s">
         <v>213</v>
       </c>
@@ -7730,7 +7761,7 @@
       <c r="O230" s="30"/>
       <c r="P230" s="1"/>
     </row>
-    <row r="231" spans="1:16">
+    <row r="231" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A231" s="9" t="s">
         <v>64</v>
       </c>
@@ -7754,7 +7785,7 @@
       </c>
       <c r="P231" s="1"/>
     </row>
-    <row r="232" spans="1:16">
+    <row r="232" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A232" s="9" t="s">
         <v>32</v>
       </c>
@@ -7778,7 +7809,7 @@
       <c r="O232" s="9"/>
       <c r="P232" s="1"/>
     </row>
-    <row r="233" spans="1:16">
+    <row r="233" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A233" s="2" t="s">
         <v>214</v>
       </c>
@@ -7798,7 +7829,7 @@
       <c r="O233" s="30"/>
       <c r="P233" s="1"/>
     </row>
-    <row r="234" spans="1:16">
+    <row r="234" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A234" s="2" t="s">
         <v>215</v>
       </c>
@@ -7818,7 +7849,7 @@
       <c r="O234" s="30"/>
       <c r="P234" s="1"/>
     </row>
-    <row r="235" spans="1:16">
+    <row r="235" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A235" s="2" t="s">
         <v>216</v>
       </c>
@@ -7838,7 +7869,7 @@
       <c r="O235" s="30"/>
       <c r="P235" s="1"/>
     </row>
-    <row r="236" spans="1:16">
+    <row r="236" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A236" s="2" t="s">
         <v>217</v>
       </c>
@@ -7858,7 +7889,7 @@
       <c r="O236" s="30"/>
       <c r="P236" s="1"/>
     </row>
-    <row r="237" spans="1:16">
+    <row r="237" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A237" s="2" t="s">
         <v>218</v>
       </c>
@@ -7895,10 +7926,12 @@
       <c r="N237" s="8">
         <v>1.3599999999999999</v>
       </c>
-      <c r="O237" s="9"/>
+      <c r="O237" s="9">
+        <v>1.18</v>
+      </c>
       <c r="P237" s="1"/>
     </row>
-    <row r="238" spans="1:16">
+    <row r="238" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A238" s="16" t="s">
         <v>219</v>
       </c>
@@ -7928,7 +7961,7 @@
       </c>
       <c r="P238" s="1"/>
     </row>
-    <row r="239" spans="1:16">
+    <row r="239" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A239" s="16"/>
       <c r="B239" s="16"/>
       <c r="C239" s="16"/>
@@ -7954,7 +7987,7 @@
       <c r="O239" s="9"/>
       <c r="P239" s="1"/>
     </row>
-    <row r="240" spans="1:16">
+    <row r="240" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A240" s="2" t="s">
         <v>220</v>
       </c>
@@ -7992,10 +8025,12 @@
       <c r="N240" s="8">
         <v>6</v>
       </c>
-      <c r="O240" s="9"/>
+      <c r="O240" s="9">
+        <v>55</v>
+      </c>
       <c r="P240" s="1"/>
     </row>
-    <row r="241" spans="1:16">
+    <row r="241" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A241" s="9" t="s">
         <v>64</v>
       </c>
@@ -8021,7 +8056,7 @@
       </c>
       <c r="P241" s="1"/>
     </row>
-    <row r="242" spans="1:16">
+    <row r="242" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A242" s="9" t="s">
         <v>32</v>
       </c>
@@ -8049,7 +8084,7 @@
       <c r="O242" s="9"/>
       <c r="P242" s="1"/>
     </row>
-    <row r="243" spans="1:16">
+    <row r="243" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A243" s="2" t="s">
         <v>221</v>
       </c>
@@ -8069,7 +8104,7 @@
       <c r="O243" s="9"/>
       <c r="P243" s="1"/>
     </row>
-    <row r="244" spans="1:16">
+    <row r="244" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A244" s="2" t="s">
         <v>222</v>
       </c>
@@ -8103,7 +8138,7 @@
       </c>
       <c r="P244" s="1"/>
     </row>
-    <row r="245" spans="1:16">
+    <row r="245" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A245" s="9" t="s">
         <v>64</v>
       </c>
@@ -8133,7 +8168,7 @@
       <c r="O245" s="9"/>
       <c r="P245" s="1"/>
     </row>
-    <row r="246" spans="1:16">
+    <row r="246" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A246" s="9" t="s">
         <v>32</v>
       </c>
@@ -8161,7 +8196,7 @@
       <c r="O246" s="9"/>
       <c r="P246" s="1"/>
     </row>
-    <row r="247" spans="1:16">
+    <row r="247" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A247" s="2" t="s">
         <v>223</v>
       </c>
@@ -8181,7 +8216,7 @@
       <c r="O247" s="9"/>
       <c r="P247" s="1"/>
     </row>
-    <row r="248" spans="1:16">
+    <row r="248" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A248" s="2" t="s">
         <v>224</v>
       </c>
@@ -8201,7 +8236,7 @@
       <c r="O248" s="9"/>
       <c r="P248" s="1"/>
     </row>
-    <row r="249" spans="1:16">
+    <row r="249" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A249" s="2" t="s">
         <v>225</v>
       </c>
@@ -8231,7 +8266,7 @@
       </c>
       <c r="P249" s="1"/>
     </row>
-    <row r="250" spans="1:16">
+    <row r="250" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A250" s="9" t="s">
         <v>64</v>
       </c>
@@ -8257,7 +8292,7 @@
       <c r="O250" s="9"/>
       <c r="P250" s="1"/>
     </row>
-    <row r="251" spans="1:16">
+    <row r="251" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A251" s="9" t="s">
         <v>32</v>
       </c>
@@ -8281,7 +8316,7 @@
       <c r="O251" s="9"/>
       <c r="P251" s="1"/>
     </row>
-    <row r="252" spans="1:16">
+    <row r="252" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A252" s="2" t="s">
         <v>226</v>
       </c>
@@ -8301,9 +8336,9 @@
       <c r="O252" s="9"/>
       <c r="P252" s="1"/>
     </row>
-    <row r="253" spans="1:16">
+    <row r="253" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A253" s="2" t="s">
-        <v>227</v>
+        <v>244</v>
       </c>
       <c r="B253" s="2"/>
       <c r="C253" s="2"/>
@@ -8321,9 +8356,9 @@
       <c r="O253" s="9"/>
       <c r="P253" s="1"/>
     </row>
-    <row r="254" spans="1:16">
+    <row r="254" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A254" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B254" s="2"/>
       <c r="C254" s="2"/>
@@ -8341,9 +8376,9 @@
       <c r="O254" s="9"/>
       <c r="P254" s="1"/>
     </row>
-    <row r="255" spans="1:16">
+    <row r="255" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A255" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B255" s="2"/>
       <c r="C255" s="2"/>
@@ -8361,9 +8396,9 @@
       <c r="O255" s="9"/>
       <c r="P255" s="1"/>
     </row>
-    <row r="256" spans="1:16">
+    <row r="256" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A256" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B256" s="2"/>
       <c r="C256" s="2"/>
@@ -8381,9 +8416,9 @@
       <c r="O256" s="9"/>
       <c r="P256" s="1"/>
     </row>
-    <row r="257" spans="1:16">
+    <row r="257" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A257" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B257" s="2"/>
       <c r="C257" s="2"/>
@@ -8401,9 +8436,9 @@
       <c r="O257" s="9"/>
       <c r="P257" s="1"/>
     </row>
-    <row r="258" spans="1:16">
+    <row r="258" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A258" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B258" s="2"/>
       <c r="C258" s="2"/>
@@ -8421,9 +8456,9 @@
       <c r="O258" s="9"/>
       <c r="P258" s="1"/>
     </row>
-    <row r="259" spans="1:16">
+    <row r="259" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A259" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B259" s="2"/>
       <c r="C259" s="2"/>
@@ -8441,9 +8476,9 @@
       <c r="O259" s="9"/>
       <c r="P259" s="1"/>
     </row>
-    <row r="260" spans="1:16">
+    <row r="260" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A260" s="2" t="s">
-        <v>234</v>
+        <v>243</v>
       </c>
       <c r="B260" s="2"/>
       <c r="C260" s="2"/>
@@ -8461,9 +8496,9 @@
       <c r="O260" s="9"/>
       <c r="P260" s="1"/>
     </row>
-    <row r="261" spans="1:16">
+    <row r="261" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A261" s="2" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
       <c r="B261" s="2"/>
       <c r="C261" s="2"/>
@@ -8481,9 +8516,9 @@
       <c r="O261" s="9"/>
       <c r="P261" s="1"/>
     </row>
-    <row r="262" spans="1:16">
+    <row r="262" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A262" s="39" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="B262" s="40"/>
       <c r="C262" s="40"/>
@@ -8523,7 +8558,7 @@
       </c>
       <c r="P262" s="1"/>
     </row>
-    <row r="263" spans="1:16">
+    <row r="263" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A263" s="9" t="s">
         <v>64</v>
       </c>
@@ -8553,7 +8588,7 @@
       <c r="O263" s="9"/>
       <c r="P263" s="1"/>
     </row>
-    <row r="264" spans="1:16">
+    <row r="264" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A264" s="9" t="s">
         <v>32</v>
       </c>
@@ -8585,9 +8620,9 @@
       <c r="O264" s="9"/>
       <c r="P264" s="1"/>
     </row>
-    <row r="265" spans="1:16">
+    <row r="265" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A265" s="2" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B265" s="2"/>
       <c r="C265" s="2"/>
@@ -8605,9 +8640,9 @@
       <c r="O265" s="9"/>
       <c r="P265" s="1"/>
     </row>
-    <row r="266" spans="1:16">
+    <row r="266" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A266" s="2" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B266" s="2"/>
       <c r="C266" s="2"/>
@@ -8625,9 +8660,9 @@
       <c r="O266" s="9"/>
       <c r="P266" s="1"/>
     </row>
-    <row r="267" spans="1:16">
+    <row r="267" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A267" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="B267" s="2"/>
       <c r="C267" s="2"/>
@@ -8645,9 +8680,9 @@
       <c r="O267" s="9"/>
       <c r="P267" s="1"/>
     </row>
-    <row r="268" spans="1:16">
+    <row r="268" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A268" s="2" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="B268" s="2"/>
       <c r="C268" s="2"/>
@@ -8665,9 +8700,9 @@
       <c r="O268" s="9"/>
       <c r="P268" s="1"/>
     </row>
-    <row r="269" spans="1:16">
+    <row r="269" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A269" s="2" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="B269" s="2"/>
       <c r="C269" s="2"/>
@@ -8691,7 +8726,7 @@
       </c>
       <c r="P269" s="1"/>
     </row>
-    <row r="270" spans="1:16">
+    <row r="270" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A270" s="9" t="s">
         <v>32</v>
       </c>
@@ -8715,9 +8750,9 @@
       <c r="O270" s="9"/>
       <c r="P270" s="1"/>
     </row>
-    <row r="271" spans="1:16">
+    <row r="271" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A271" s="9" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="B271" s="9"/>
       <c r="C271" s="9"/>
@@ -8737,9 +8772,9 @@
       <c r="O271" s="9"/>
       <c r="P271" s="1"/>
     </row>
-    <row r="272" spans="1:16">
+    <row r="272" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A272" s="2" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="B272" s="2"/>
       <c r="C272" s="2"/>
@@ -8757,9 +8792,9 @@
       <c r="O272" s="9"/>
       <c r="P272" s="1"/>
     </row>
-    <row r="273" spans="1:16">
+    <row r="273" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A273" s="2" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="B273" s="2"/>
       <c r="C273" s="2"/>
@@ -8777,9 +8812,9 @@
       <c r="O273" s="9"/>
       <c r="P273" s="1"/>
     </row>
-    <row r="274" spans="1:16">
+    <row r="274" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A274" s="2" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="B274" s="2"/>
       <c r="C274" s="2"/>
@@ -8814,6 +8849,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="dokument" ma:contentTypeID="0x010100A3F2E6F3B9C90048992043A88C54C6CD" ma:contentTypeVersion="2" ma:contentTypeDescription="Skapa ett nytt dokument." ma:contentTypeScope="" ma:versionID="5aebe702395f3f48d5109754cd6a3069">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="584d8bbe-a375-40d4-8b82-cbb9642a2964" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4b4574b0081c16b734b0cc75f42d1b75" ns2:_="">
     <xsd:import namespace="584d8bbe-a375-40d4-8b82-cbb9642a2964"/>
@@ -8945,12 +8986,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -8961,13 +8996,36 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A598D07-ACF3-49CF-823D-C653630475F5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D263FA3-831D-4878-BA57-1292F567598F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D263FA3-831D-4878-BA57-1292F567598F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A598D07-ACF3-49CF-823D-C653630475F5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="584d8bbe-a375-40d4-8b82-cbb9642a2964"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66331DBF-6ADD-497C-87DE-0B19F327D7B5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66331DBF-6ADD-497C-87DE-0B19F327D7B5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
16/01 - Final commit, end of the road
</commit_message>
<xml_diff>
--- a/Manufacturing.xlsx
+++ b/Manufacturing.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucar\PycharmProjects\NJORD_2022_Albin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F22FFAAD-A141-4B9A-A1C3-56190C62D5AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7591E8D5-AAC7-4265-8F56-D0F3566F239F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{25E8C77A-571D-440B-A5FA-B562A92F21E1}"/>
   </bookViews>
@@ -2346,8 +2346,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463DEAE1-12B4-4B7D-A82D-D43D3DD59FCF}">
   <dimension ref="A1:V274"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A251" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="A268" sqref="A268"/>
+    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2732,7 +2732,9 @@
       <c r="O14" s="9">
         <v>35</v>
       </c>
-      <c r="P14" s="1"/>
+      <c r="P14" s="1">
+        <v>35</v>
+      </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
@@ -2826,7 +2828,9 @@
       <c r="O17" s="9">
         <v>134</v>
       </c>
-      <c r="P17" s="1"/>
+      <c r="P17" s="1">
+        <v>134</v>
+      </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
@@ -3029,8 +3033,12 @@
       <c r="N26" s="8">
         <v>11</v>
       </c>
-      <c r="O26" s="9"/>
-      <c r="P26" s="1"/>
+      <c r="O26" s="9">
+        <v>11</v>
+      </c>
+      <c r="P26" s="1">
+        <v>11</v>
+      </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
@@ -3611,7 +3619,9 @@
       <c r="O51" s="9">
         <v>1430</v>
       </c>
-      <c r="P51" s="1"/>
+      <c r="P51" s="1">
+        <v>1430</v>
+      </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A52" s="9" t="s">
@@ -3789,7 +3799,9 @@
       <c r="O58" s="9">
         <v>124600</v>
       </c>
-      <c r="P58" s="1"/>
+      <c r="P58" s="1">
+        <v>124600</v>
+      </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A59" s="9" t="s">
@@ -4408,8 +4420,12 @@
       <c r="N86" s="8">
         <v>6.25</v>
       </c>
-      <c r="O86" s="9"/>
-      <c r="P86" s="1"/>
+      <c r="O86" s="9">
+        <v>6.25</v>
+      </c>
+      <c r="P86" s="1">
+        <v>6.25</v>
+      </c>
     </row>
     <row r="87" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A87" s="9" t="s">
@@ -4471,7 +4487,9 @@
       <c r="O88" s="9">
         <v>840</v>
       </c>
-      <c r="P88" s="1"/>
+      <c r="P88" s="1">
+        <v>840</v>
+      </c>
     </row>
     <row r="89" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A89" s="9" t="s">
@@ -4646,8 +4664,12 @@
       <c r="N95" s="19">
         <v>900</v>
       </c>
-      <c r="O95" s="20"/>
-      <c r="P95" s="1"/>
+      <c r="O95" s="20">
+        <v>900</v>
+      </c>
+      <c r="P95" s="1">
+        <v>900</v>
+      </c>
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A96" s="9" t="s">
@@ -5065,7 +5087,9 @@
       <c r="O114" s="20">
         <v>920</v>
       </c>
-      <c r="P114" s="1"/>
+      <c r="P114" s="1">
+        <v>920</v>
+      </c>
     </row>
     <row r="115" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A115" s="24" t="s">
@@ -5232,7 +5256,9 @@
       <c r="O121" s="9">
         <v>75.2</v>
       </c>
-      <c r="P121" s="1"/>
+      <c r="P121" s="1">
+        <v>75.2</v>
+      </c>
     </row>
     <row r="122" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A122" s="9" t="s">
@@ -5369,7 +5395,9 @@
       <c r="O126" s="9">
         <v>600</v>
       </c>
-      <c r="P126" s="1"/>
+      <c r="P126" s="1">
+        <v>700</v>
+      </c>
     </row>
     <row r="127" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A127" s="9" t="s">
@@ -8556,7 +8584,9 @@
       <c r="O262" s="9">
         <v>3250</v>
       </c>
-      <c r="P262" s="1"/>
+      <c r="P262" s="1">
+        <v>3250</v>
+      </c>
     </row>
     <row r="263" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A263" s="9" t="s">
@@ -8724,7 +8754,9 @@
       <c r="O269" s="9">
         <v>14130</v>
       </c>
-      <c r="P269" s="1"/>
+      <c r="P269" s="1">
+        <v>14130</v>
+      </c>
     </row>
     <row r="270" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A270" s="9" t="s">
@@ -8849,9 +8881,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8987,19 +9022,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D263FA3-831D-4878-BA57-1292F567598F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66331DBF-6ADD-497C-87DE-0B19F327D7B5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9023,9 +9054,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66331DBF-6ADD-497C-87DE-0B19F327D7B5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D263FA3-831D-4878-BA57-1292F567598F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>